<commit_message>
modify cache size to 5
</commit_message>
<xml_diff>
--- a/hw2_requirements.xlsx
+++ b/hw2_requirements.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\brandon\HTTP_Caching_Proxy\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E38D38-33C9-4018-8971-82AC3B1950B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="16480"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>Extra note to TA</t>
   </si>
@@ -82,19 +88,16 @@
   </si>
   <si>
     <t>Any extra tests you would like to mention?</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -137,24 +140,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
@@ -458,28 +458,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="64.1640625" customWidth="1"/>
+    <col min="1" max="1" width="64.1328125" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="62.83203125" customWidth="1"/>
+    <col min="3" max="3" width="62.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24">
+    <row r="1" spans="1:3" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -490,106 +490,141 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" customHeight="1">
+    <row r="2" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5"/>
-    </row>
-    <row r="3" spans="1:3" ht="16" customHeight="1">
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5"/>
-    </row>
-    <row r="4" spans="1:3" ht="16" customHeight="1">
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5"/>
-    </row>
-    <row r="5" spans="1:3" ht="16" customHeight="1">
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" ht="16" customHeight="1">
+      <c r="B5" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="1:3" ht="16" customHeight="1">
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" ht="16" customHeight="1">
+      <c r="B7" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="5"/>
-    </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1">
+      <c r="B8" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:3" ht="16" customHeight="1">
+    <row r="10" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="5"/>
-    </row>
-    <row r="11" spans="1:3" ht="16" customHeight="1">
+      <c r="B10" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:3" ht="55" customHeight="1">
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="55.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" ht="16" customHeight="1">
+      <c r="B12" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:3" ht="16" customHeight="1">
+      <c r="B13" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="5"/>
-    </row>
-    <row r="15" spans="1:3" ht="43" customHeight="1">
+      <c r="B14" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="43.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="5"/>
-    </row>
-    <row r="16" spans="1:3" ht="31" customHeight="1">
+      <c r="B15" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="31.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" ht="16" customHeight="1">
+      <c r="B16" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" ht="16" customHeight="1">
+      <c r="B17" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" ht="16" customHeight="1">
+      <c r="B18" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="16.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
set limitation for cache size to 10 MB
</commit_message>
<xml_diff>
--- a/hw2_requirements.xlsx
+++ b/hw2_requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\brandon\HTTP_Caching_Proxy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB20B30-FA8D-4A14-87F9-295150E61362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E582A936-5E42-4D4D-80EE-853918D11CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,7 +93,7 @@
     <t>Y</t>
   </si>
   <si>
-    <t xml:space="preserve">We use the First In First Out replacement policy, which acts like a queue, the first stored response will be removed if the capacity is full. And we set the capacity to 5 because it is easier to test. The expired response will be cleaned when a new request from the client asks for it. </t>
+    <t xml:space="preserve">The limitation of every cache is 10 MB. We use the First In First Out replacement policy, which acts like a queue, the first stored response will be removed if the capacity is full. And we set the capacity to 5 because it is easier to test. The expired response will be cleaned when a new request from the client asks for it. </t>
   </si>
 </sst>
 </file>
@@ -472,7 +472,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>